<commit_message>
register page full update
</commit_message>
<xml_diff>
--- a/src/test/resources/bashData.xlsx
+++ b/src/test/resources/bashData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d5ec3308cc1e089/Desktop/Ecommerce/bashAutomation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{CF8D9E6D-23A4-469D-9EEE-B76D02C7EBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5852BD5-25FC-42E1-B14A-A8256DCCB8AE}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{CF8D9E6D-23A4-469D-9EEE-B76D02C7EBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3935F819-AE02-4455-90BF-B18E6D0E8B00}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C0B666EE-EB63-493E-92DB-F30BEF9B9009}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>S.N</t>
   </si>
@@ -48,9 +49,6 @@
     <t>DataKey1</t>
   </si>
   <si>
-    <t>DataVAlue1</t>
-  </si>
-  <si>
     <t>UserNameID</t>
   </si>
   <si>
@@ -63,9 +61,6 @@
     <t>Bash001</t>
   </si>
   <si>
-    <t>verifyBash001SearchProducts</t>
-  </si>
-  <si>
     <t>DataValue2</t>
   </si>
   <si>
@@ -87,9 +82,6 @@
     <t>Hello, RK</t>
   </si>
   <si>
-    <t>verifyBash002SNewUserRegister</t>
-  </si>
-  <si>
     <t>Bash002</t>
   </si>
   <si>
@@ -105,9 +97,6 @@
     <t>munna</t>
   </si>
   <si>
-    <t>DataValye4</t>
-  </si>
-  <si>
     <t>DataValue4</t>
   </si>
   <si>
@@ -115,25 +104,67 @@
   </si>
   <si>
     <t>Yadav</t>
+  </si>
+  <si>
+    <t>DataValue1</t>
+  </si>
+  <si>
+    <t>DataKey4</t>
+  </si>
+  <si>
+    <t>verifyBash001SNewUserRegister</t>
+  </si>
+  <si>
+    <t>verifyBash006ValidDeatilsUserLogin</t>
+  </si>
+  <si>
+    <t>Bash006</t>
+  </si>
+  <si>
+    <t>verifyBash004RegisterWithApple</t>
+  </si>
+  <si>
+    <t>Bash004</t>
+  </si>
+  <si>
+    <t>Bash003</t>
+  </si>
+  <si>
+    <t>AppleTextHearder</t>
+  </si>
+  <si>
+    <t>Apple Account</t>
+  </si>
+  <si>
+    <t>FaceBookTextHearder</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>verifyBash003RegisterWithfaceBook</t>
+  </si>
+  <si>
+    <t>verifyBash002RegisterWithGoogle</t>
+  </si>
+  <si>
+    <t>GoogleTextHearder</t>
+  </si>
+  <si>
+    <t>Sign in with Google</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <u/>
@@ -157,12 +188,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,19 +216,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,20 +253,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,180 +589,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8881D1E9-5B57-44B6-943C-248072C3587A}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="41.6328125" customWidth="1"/>
     <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="22.36328125" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" customWidth="1"/>
-    <col min="11" max="11" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18" style="4" customWidth="1"/>
+    <col min="8" max="8" width="22.36328125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="14.36328125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="4"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I9" s="9"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{4565655F-35F8-46DA-8971-55B911101759}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{4C244EEF-C394-475A-8F41-12E97C184C16}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{4565655F-35F8-46DA-8971-55B911101759}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{4C244EEF-C394-475A-8F41-12E97C184C16}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316887AF-4D7E-42CC-B334-1E32BF426A64}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>